<commit_message>
implement data preprocessing, na-screening visualization, na-screening traffic and 3D plots plus modification
</commit_message>
<xml_diff>
--- a/data/cleaned/cw_T1_cleaned.xlsx
+++ b/data/cleaned/cw_T1_cleaned.xlsx
@@ -646,7 +646,7 @@
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>nitrite</t>
+          <t>nitrite - N</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>nitrate</t>
+          <t>nitrate - N</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">

</xml_diff>